<commit_message>
Added AddressRange Commands Added MulticastAddressRange Commands Added GroupWithExclusion Commands Added SecurityZone Commands
</commit_message>
<xml_diff>
--- a/Examples/ImportExcel/Import.xlsx
+++ b/Examples/ImportExcel/Import.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tim\Source\Repos\psCheckPoint\Examples\ImportExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tim\source\repos\psCheckPoint\Examples\ImportExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="2" r:id="rId1"/>
-    <sheet name="Hosts" sheetId="3" r:id="rId2"/>
-    <sheet name="Networks" sheetId="4" r:id="rId3"/>
+    <sheet name="Groups with Exclusion" sheetId="7" r:id="rId2"/>
+    <sheet name="Hosts" sheetId="3" r:id="rId3"/>
+    <sheet name="Networks" sheetId="4" r:id="rId4"/>
+    <sheet name="Address Ranges" sheetId="5" r:id="rId5"/>
+    <sheet name="Multicast Address Ranges" sheetId="6" r:id="rId6"/>
+    <sheet name="Security Zones" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -155,6 +159,117 @@
   </si>
   <si>
     <t>Tags Rule;Really Rule</t>
+  </si>
+  <si>
+    <t>IPAddressFirst</t>
+  </si>
+  <si>
+    <t>IPAddressLast</t>
+  </si>
+  <si>
+    <t>IPv4AddressFirst</t>
+  </si>
+  <si>
+    <t>IPv4AddressLast</t>
+  </si>
+  <si>
+    <t>IPv6AddressFirst</t>
+  </si>
+  <si>
+    <t>IPv6AddressLast</t>
+  </si>
+  <si>
+    <t>TestAR1</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>Another Tag</t>
+  </si>
+  <si>
+    <t>Testing 123, Testing</t>
+  </si>
+  <si>
+    <t>TestAR2</t>
+  </si>
+  <si>
+    <t>192.168.0.0</t>
+  </si>
+  <si>
+    <t>192.168.255.255</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>Tag Your it</t>
+  </si>
+  <si>
+    <t>TestAR3</t>
+  </si>
+  <si>
+    <t>10.1.2.3</t>
+  </si>
+  <si>
+    <t>10.4.5.6</t>
+  </si>
+  <si>
+    <t>fd00:1234::1000</t>
+  </si>
+  <si>
+    <t>10.255.255.255</t>
+  </si>
+  <si>
+    <t>TestMAR1</t>
+  </si>
+  <si>
+    <t>224.0.0.0</t>
+  </si>
+  <si>
+    <t>239.255.255.255</t>
+  </si>
+  <si>
+    <t>Multicast</t>
+  </si>
+  <si>
+    <t>TestMAR2</t>
+  </si>
+  <si>
+    <t>225.6.7.8</t>
+  </si>
+  <si>
+    <t>224.5.6.7</t>
+  </si>
+  <si>
+    <t>FF01:0:0:0:0:0:0:1</t>
+  </si>
+  <si>
+    <t>FF01:0:0:0:0:0:0:2</t>
+  </si>
+  <si>
+    <t>TestMAR3</t>
+  </si>
+  <si>
+    <t>FF05:0:0:0:0:0:0:2</t>
+  </si>
+  <si>
+    <t>Single Multiecast IP</t>
+  </si>
+  <si>
+    <t>TestGroupExclude</t>
+  </si>
+  <si>
+    <t>Include</t>
+  </si>
+  <si>
+    <t>Except</t>
+  </si>
+  <si>
+    <t>TestSZ1</t>
+  </si>
+  <si>
+    <t>TestSZ2</t>
   </si>
 </sst>
 </file>
@@ -572,11 +687,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADB3CE1-A5BD-4427-B7A3-E9462001754A}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,12 +859,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,4 +978,294 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB069E9-CCE0-4B35-A690-4EE74665EDE5}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB95F9E-D633-40EC-82A1-39D29C5792D4}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904A022D-2F92-477B-A539-0D9DD4B2332A}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
First take of ExportCheckPointAccessRule
</commit_message>
<xml_diff>
--- a/Examples/ImportExcel/Import.xlsx
+++ b/Examples/ImportExcel/Import.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Address Ranges" sheetId="5" r:id="rId5"/>
     <sheet name="Multicast Address Ranges" sheetId="6" r:id="rId6"/>
     <sheet name="Security Zones" sheetId="8" r:id="rId7"/>
+    <sheet name="Access Layers" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -270,6 +271,33 @@
   </si>
   <si>
     <t>TestSZ2</t>
+  </si>
+  <si>
+    <t>AddDefaultRule</t>
+  </si>
+  <si>
+    <t>ApplicationsAndUrlFiltering</t>
+  </si>
+  <si>
+    <t>ContentAwareness</t>
+  </si>
+  <si>
+    <t>DetectUsingXForwardFor</t>
+  </si>
+  <si>
+    <t>Firewall</t>
+  </si>
+  <si>
+    <t>MobileAccess</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>TestAccessLayer1</t>
+  </si>
+  <si>
+    <t>TestAccessLayer2</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904A022D-2F92-477B-A539-0D9DD4B2332A}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1268,4 +1296,95 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B3E7B9-4DE0-4101-9E39-4974B994A9DE}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="40.85546875" customWidth="1"/>
+    <col min="11" max="11" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Allow Nulls to assist with imports
</commit_message>
<xml_diff>
--- a/Examples/ImportExcel/Import.xlsx
+++ b/Examples/ImportExcel/Import.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tim\source\repos\psCheckPoint\Examples\ImportExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KoopmanT\source\repos\psCheckPoint\Examples\ImportExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,6 @@
     <sheet name="Networks" sheetId="4" r:id="rId4"/>
     <sheet name="Address Ranges" sheetId="5" r:id="rId5"/>
     <sheet name="Multicast Address Ranges" sheetId="6" r:id="rId6"/>
-    <sheet name="Security Zones" sheetId="8" r:id="rId7"/>
-    <sheet name="Access Layers" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -48,12 +46,6 @@
     <t>Groups</t>
   </si>
   <si>
-    <t>Subnet</t>
-  </si>
-  <si>
-    <t>MaskLength</t>
-  </si>
-  <si>
     <t>TestGroupA</t>
   </si>
   <si>
@@ -93,24 +85,15 @@
     <t>192.168.2.1</t>
   </si>
   <si>
-    <t>TestHostD</t>
-  </si>
-  <si>
     <t>TestNetworkA</t>
   </si>
   <si>
-    <t>192.168.1.0</t>
-  </si>
-  <si>
     <t>Comment me</t>
   </si>
   <si>
     <t>TestNetworkB</t>
   </si>
   <si>
-    <t>192.168.2.0</t>
-  </si>
-  <si>
     <t>TestNetworkC</t>
   </si>
   <si>
@@ -126,15 +109,6 @@
     <t>fd00:1234::1</t>
   </si>
   <si>
-    <t>fd00:1234::2</t>
-  </si>
-  <si>
-    <t>SubnetMask</t>
-  </si>
-  <si>
-    <t>255.255.255.128</t>
-  </si>
-  <si>
     <t>Subnet4</t>
   </si>
   <si>
@@ -150,9 +124,6 @@
     <t>fd00::</t>
   </si>
   <si>
-    <t>IPAddress</t>
-  </si>
-  <si>
     <t>IPv4Address</t>
   </si>
   <si>
@@ -162,12 +133,6 @@
     <t>Tags Rule;Really Rule</t>
   </si>
   <si>
-    <t>IPAddressFirst</t>
-  </si>
-  <si>
-    <t>IPAddressLast</t>
-  </si>
-  <si>
     <t>IPv4AddressFirst</t>
   </si>
   <si>
@@ -186,12 +151,6 @@
     <t>red</t>
   </si>
   <si>
-    <t>Another Tag</t>
-  </si>
-  <si>
-    <t>Testing 123, Testing</t>
-  </si>
-  <si>
     <t>TestAR2</t>
   </si>
   <si>
@@ -207,9 +166,6 @@
     <t>Tag Your it</t>
   </si>
   <si>
-    <t>TestAR3</t>
-  </si>
-  <si>
     <t>10.1.2.3</t>
   </si>
   <si>
@@ -219,9 +175,6 @@
     <t>fd00:1234::1000</t>
   </si>
   <si>
-    <t>10.255.255.255</t>
-  </si>
-  <si>
     <t>TestMAR1</t>
   </si>
   <si>
@@ -237,21 +190,12 @@
     <t>TestMAR2</t>
   </si>
   <si>
-    <t>225.6.7.8</t>
-  </si>
-  <si>
-    <t>224.5.6.7</t>
-  </si>
-  <si>
     <t>FF01:0:0:0:0:0:0:1</t>
   </si>
   <si>
     <t>FF01:0:0:0:0:0:0:2</t>
   </si>
   <si>
-    <t>TestMAR3</t>
-  </si>
-  <si>
     <t>FF05:0:0:0:0:0:0:2</t>
   </si>
   <si>
@@ -265,45 +209,12 @@
   </si>
   <si>
     <t>Except</t>
-  </si>
-  <si>
-    <t>TestSZ1</t>
-  </si>
-  <si>
-    <t>TestSZ2</t>
-  </si>
-  <si>
-    <t>AddDefaultRule</t>
-  </si>
-  <si>
-    <t>ApplicationsAndUrlFiltering</t>
-  </si>
-  <si>
-    <t>ContentAwareness</t>
-  </si>
-  <si>
-    <t>DetectUsingXForwardFor</t>
-  </si>
-  <si>
-    <t>Firewall</t>
-  </si>
-  <si>
-    <t>MobileAccess</t>
-  </si>
-  <si>
-    <t>Shared</t>
-  </si>
-  <si>
-    <t>TestAccessLayer1</t>
-  </si>
-  <si>
-    <t>TestAccessLayer2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -657,11 +568,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,24 +599,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +626,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADB3CE1-A5BD-4427-B7A3-E9462001754A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -735,10 +646,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -752,22 +663,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -777,109 +688,98 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="2" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -888,119 +788,110 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="29.140625" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" customWidth="1"/>
-    <col min="12" max="12" width="33.140625" customWidth="1"/>
+    <col min="2" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C2">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="C4">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3">
-        <v>8</v>
-      </c>
-      <c r="I3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4">
-        <v>8</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1009,127 +900,96 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB069E9-CCE0-4B35-A690-4EE74665EDE5}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" t="s">
-        <v>55</v>
+      <c r="F3" t="s">
+        <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1138,253 +998,88 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB95F9E-D633-40EC-82A1-39D29C5792D4}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>63</v>
-      </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" t="s">
         <v>50</v>
       </c>
-      <c r="K2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904A022D-2F92-477B-A539-0D9DD4B2332A}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B3E7B9-4DE0-4101-9E39-4974B994A9DE}">
-  <dimension ref="A1:K3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="21.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="40.85546875" customWidth="1"/>
-    <col min="11" max="11" width="28.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>